<commit_message>
alimentando planilha batch input
</commit_message>
<xml_diff>
--- a/MODELO BATCH INPUT.xlsx
+++ b/MODELO BATCH INPUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Partes Relacionadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE61044-FA95-4F18-A3D8-2C428B5DAEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6703DE7-8A11-482D-81D1-CDA08BC1C1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B.I. (ajuste -)" sheetId="14" r:id="rId1"/>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -283,6 +283,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,33 +575,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B861854C-99BF-4EA2-9D92-68017304C3A9}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="10" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" customWidth="1"/>
-    <col min="7" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="9" customWidth="1"/>
+    <col min="7" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" customWidth="1"/>
-    <col min="21" max="21" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" customWidth="1"/>
+    <col min="21" max="21" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -605,13 +611,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -673,30 +679,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD151"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="10" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" customWidth="1"/>
-    <col min="7" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="10" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="9" customWidth="1"/>
+    <col min="7" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" customWidth="1"/>
-    <col min="21" max="21" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" customWidth="1"/>
+    <col min="21" max="21" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -706,13 +712,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -773,32 +779,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5FDD65-15A9-4EC0-A195-A7BE14996053}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD245"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="10" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" customWidth="1"/>
-    <col min="7" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="10" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" customWidth="1"/>
+    <col min="7" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" customWidth="1"/>
-    <col min="21" max="21" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" customWidth="1"/>
+    <col min="21" max="21" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -808,10 +814,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">

</xml_diff>

<commit_message>
novos ajustes a pedido do usuario
</commit_message>
<xml_diff>
--- a/MODELO BATCH INPUT.xlsx
+++ b/MODELO BATCH INPUT.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Partes Relacionadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6703DE7-8A11-482D-81D1-CDA08BC1C1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07FB2AC-F363-47E7-8BDC-E7ADF15A87E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="B.I. (ajuste -)" sheetId="14" r:id="rId1"/>
-    <sheet name="B.I. (ajuste +)" sheetId="12" r:id="rId2"/>
-    <sheet name="B.I. (intercompany)" sheetId="13" r:id="rId3"/>
+    <sheet name="B.I. Intercompany" sheetId="13" r:id="rId1"/>
+    <sheet name="B.I. Passivo" sheetId="14" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'B.I. (ajuste -)'!$V$1:$AA$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'B.I. (ajuste +)'!$A$1:$U$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'B.I. (intercompany)'!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'B.I. Intercompany'!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'B.I. Passivo'!$V$1:$AA$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Sequencial</t>
   </si>
@@ -572,6 +570,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5FDD65-15A9-4EC0-A195-A7BE14996053}">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="10" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="11" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" customWidth="1"/>
+    <col min="21" max="21" width="52.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:U1" xr:uid="{2A5F090C-236A-44DC-A72A-D4B8B3063190}"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B861854C-99BF-4EA2-9D92-68017304C3A9}">
   <dimension ref="A1:U1"/>
   <sheetViews>
@@ -580,28 +680,28 @@
       <selection pane="bottomLeft" activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="10" customWidth="1"/>
-    <col min="2" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="9" customWidth="1"/>
-    <col min="7" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="9" customWidth="1"/>
+    <col min="7" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" customWidth="1"/>
-    <col min="19" max="19" width="9.5546875" customWidth="1"/>
-    <col min="20" max="20" width="7.88671875" customWidth="1"/>
-    <col min="21" max="21" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" customWidth="1"/>
+    <col min="21" max="21" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="14" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -671,208 +771,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAF0561-014E-4AA7-AC22-543E6DA3BBC1}">
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:F1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.33203125" style="10" customWidth="1"/>
-    <col min="2" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="9" customWidth="1"/>
-    <col min="7" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" customWidth="1"/>
-    <col min="19" max="19" width="9.5546875" customWidth="1"/>
-    <col min="20" max="20" width="7.88671875" customWidth="1"/>
-    <col min="21" max="21" width="52.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:U1" xr:uid="{DCAF0561-014E-4AA7-AC22-543E6DA3BBC1}"/>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5FDD65-15A9-4EC0-A195-A7BE14996053}">
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.33203125" style="10" customWidth="1"/>
-    <col min="2" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" customWidth="1"/>
-    <col min="7" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" style="11" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" customWidth="1"/>
-    <col min="19" max="19" width="9.5546875" customWidth="1"/>
-    <col min="20" max="20" width="7.88671875" customWidth="1"/>
-    <col min="21" max="21" width="52.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:U1" xr:uid="{2A5F090C-236A-44DC-A72A-D4B8B3063190}"/>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>